<commit_message>
Updated Rev0 PCB Release
PPU2 paste removed
Pin connector paste removed
Altium Releaser still does not work properly
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for SNES TST Adapter/Rev 0/Assembly/Type A/Bill of Materials-SNES TST Adapter(SNES TST Adapter).xlsx
+++ b/PCB/Project Outputs for SNES TST Adapter/Rev 0/Assembly/Type A/Bill of Materials-SNES TST Adapter(SNES TST Adapter).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ft\AppData\Local\TempReleases\Snapshot\2\Assembly SNES TST Adapter\Type A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ft\AppData\Local\TempReleases\Snapshot\3\Assembly SNES TST Adapter\Type A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C64441C-D394-4C52-97B6-EB931D29C487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58CDCEF6-8D6C-46BF-BA1D-4CBECA1E2E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="585" xr2:uid="{7457765A-D0DB-4BF1-B0E4-6BDADA15CE41}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="585" xr2:uid="{3EB4AEDD-2EBF-49E9-B993-2752CC94C0A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-SNES TST Adap" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EFACB7-D2DF-4EB0-8508-9928F60C0353}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C371850-F007-45C4-995E-F14D4D2BE4C6}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>